<commit_message>
cleaned up script + created copy of dict
</commit_message>
<xml_diff>
--- a/pH_optode/lab_cs_instruments_config_mock.xlsx
+++ b/pH_optode/lab_cs_instruments_config_mock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/Github/lab_work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/lab-work/pH_optode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17C89844-E2EE-41B2-B50F-AC06F1B5AF26}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{03E158C2-E06C-4FDE-9F94-B1C35A89DB2A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>batch</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>30072020_J1</t>
   </si>
   <si>
     <t>pH_optN</t>
@@ -524,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24354337-39CE-416A-A127-42BEC72437C4}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,7 +567,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -634,7 +631,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -694,12 +691,12 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.35">
@@ -710,11 +707,6 @@
     <row r="18" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K18" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K19" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -725,6 +717,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027E85BF46FFBA5448F68919BA489A1DA" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="45a9c6a0386fdd3966398fc659f672bc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211" xmlns:ns4="1e11a0bb-5c52-4e83-8dd3-aa81c1705742" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5fd16eb0bef241ffc3cb418196d56410" ns3:_="" ns4:_="">
     <xsd:import namespace="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211"/>
@@ -947,22 +954,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E16F44-C68D-4E79-A4BA-87CF7924D4A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1e11a0bb-5c52-4e83-8dd3-aa81c1705742"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77FFA200-F0B2-4031-AD08-862C0DB7F006}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46B2F9E1-9454-4E0C-80CD-4240C2750498}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -979,29 +996,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77FFA200-F0B2-4031-AD08-862C0DB7F006}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E16F44-C68D-4E79-A4BA-87CF7924D4A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1e11a0bb-5c52-4e83-8dd3-aa81c1705742"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>